<commit_message>
Adding per capita measures for migration
</commit_message>
<xml_diff>
--- a/.data/sodertornsmodellen/ddf--sodertornsmodellen--testing2016/data_process/ddf--measures.xlsx
+++ b/.data/sodertornsmodellen/ddf--sodertornsmodellen--testing2016/data_process/ddf--measures.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cjbackman/Google Drive/gapminder/sodertornsmodellen/ddf--sodertornsmodellen--testing2016/data_process/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cjbackman/work/sodertornsmodellen/ddf--sodertornsmodellen--testing2016/data_process/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="25740" windowHeight="15960"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28720" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>measure</t>
   </si>
@@ -77,12 +77,6 @@
     <t>Förvärvsintensitet är ett mått som anger andel personer med bostad i regionen (nattbefolkning) som förvärvsarbetar i en viss åldersgrupp i relation till samtliga personer i den aktuella åldersgruppen. Förvärvsintensitet beräknas ofta utifrån i åldersklassen 20-64 år eller 16-64 år.</t>
   </si>
   <si>
-    <t>Nettomigration till/från ett geografisk område på grund av arbete.</t>
-  </si>
-  <si>
-    <t>Nettomigration till/från ett geografisk område på grund av utbildning.</t>
-  </si>
-  <si>
     <t>Andel av befolkningen som har eftergymnasial utbildning (3+ år).</t>
   </si>
   <si>
@@ -90,6 +84,24 @@
   </si>
   <si>
     <t>Medelinkomsten i ett givet geografiskt område.</t>
+  </si>
+  <si>
+    <t>Nettomigration till/från ett geografisk område (arbete).</t>
+  </si>
+  <si>
+    <t>Nettomigration till/från ett geografisk område (utbildning).</t>
+  </si>
+  <si>
+    <t>flytt_arbete_p_cap</t>
+  </si>
+  <si>
+    <t>flytt_utbildning_p_cap</t>
+  </si>
+  <si>
+    <t>Nettomigration till/från ett geografisk område (arbete) per capita.</t>
+  </si>
+  <si>
+    <t>Nettomigration till/från ett geografisk område (utbildning) per capita.</t>
   </si>
 </sst>
 </file>
@@ -454,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -487,7 +499,7 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -501,7 +513,7 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -515,7 +527,7 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -543,7 +555,7 @@
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -557,7 +569,35 @@
         <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>